<commit_message>
Design documentation update only
</commit_message>
<xml_diff>
--- a/docs/Requirements.xlsx
+++ b/docs/Requirements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://europro365-my.sharepoint.com/personal/bbiring_sharkninja_com/Documents/Python - CostWalk/CostWalkPythonProject/documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\ElectricalBomAnalyser\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="13_ncr:1_{5B59A0DE-2980-4BC7-9800-86D273F60FA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A93F7D6F-5BDC-418B-9CA5-7DC0A68A9273}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2621701B-3E11-4667-A555-7309A7E53DB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15150" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{CD613DC0-3E3F-45D7-9A81-B6EDC2BEC512}"/>
+    <workbookView xWindow="-15150" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CD613DC0-3E3F-45D7-9A81-B6EDC2BEC512}"/>
   </bookViews>
   <sheets>
     <sheet name="Need" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
   <si>
     <t>Source</t>
   </si>
@@ -59,9 +59,6 @@
     <t>The application shall read data from the costed bill of material excel data</t>
   </si>
   <si>
-    <t>As the user, I want to analyse the product cost by grouping components by feature</t>
-  </si>
-  <si>
     <t>As the user, I want to compare the product featue cost change from one build to another</t>
   </si>
   <si>
@@ -83,9 +80,6 @@
     <t>Title</t>
   </si>
   <si>
-    <t>Read excel CBOM</t>
-  </si>
-  <si>
     <t>Feature cost</t>
   </si>
   <si>
@@ -107,14 +101,124 @@
     <t>As the user, I want to plot feature cost change from one build to another</t>
   </si>
   <si>
-    <t>As the user, I want to use the costed bill of material to analyse product cost</t>
+    <t>As the user, I want to use the costed bill of material to analyse electrical cost</t>
+  </si>
+  <si>
+    <t>Excel CBOM</t>
+  </si>
+  <si>
+    <t>As the user, I want to analyse the electrical product cost by grouping components by feature</t>
+  </si>
+  <si>
+    <t>Failure Mode</t>
+  </si>
+  <si>
+    <t>Failure Effect</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Detection
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>10 = None
+1 = Absolute</t>
+    </r>
+  </si>
+  <si>
+    <t>RPN</t>
+  </si>
+  <si>
+    <t>New RPN</t>
+  </si>
+  <si>
+    <t>Failure Cause</t>
+  </si>
+  <si>
+    <t>Current Control</t>
+  </si>
+  <si>
+    <t>Recommended Detection</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Severity
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>10 = Catastrophic
+1 = insignificant</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Occurrence
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>10 = inevitable
+1 = unlikely</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">New Detection
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>10 = None
+1 = Absolute</t>
+    </r>
+  </si>
+  <si>
+    <t>user dissatisfaction</t>
+  </si>
+  <si>
+    <t>failed to analyze electrical cost</t>
+  </si>
+  <si>
+    <t>file format not recognized by the application</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>The application shall accept excell file format</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,6 +241,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -168,7 +279,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -187,6 +298,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -504,7 +627,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDAC9AAD-44E6-4961-9956-B41DD506D942}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -521,7 +644,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -532,57 +655,57 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -593,14 +716,105 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FA97F52-1176-4A3B-A8AE-B9C95F6F82D0}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="3" width="31" style="9" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" style="9" customWidth="1"/>
+    <col min="5" max="5" width="31" style="10" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" style="9" customWidth="1"/>
+    <col min="7" max="7" width="31" style="10" customWidth="1"/>
+    <col min="8" max="9" width="14.33203125" style="9" customWidth="1"/>
+    <col min="10" max="10" width="31" style="10" customWidth="1"/>
+    <col min="11" max="12" width="14.33203125" style="9" customWidth="1"/>
+    <col min="13" max="16384" width="8.88671875" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="38.4" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="str">
+        <f>Need!C2</f>
+        <v>As the user, I want to use the costed bill of material to analyse electrical cost</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="9">
+        <v>10</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="9">
+        <v>10</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" s="9">
+        <v>10</v>
+      </c>
+      <c r="I2" s="9">
+        <f>D2*F2*H2</f>
+        <v>1000</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="K2" s="9">
+        <v>1</v>
+      </c>
+      <c r="L2" s="9">
+        <f>D2*F2*K2</f>
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -634,7 +848,7 @@
     </row>
     <row r="2" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>4</v>
@@ -646,7 +860,7 @@
     </row>
     <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -684,7 +898,7 @@
   <sheetData>
     <row r="4" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -724,7 +938,7 @@
   <sheetData>
     <row r="4" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>